<commit_message>
Update RTM in Test cases Login module
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix .xlsx
+++ b/Monitor and Control/Car-Traceability Matrix .xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Car System\Github\Car-Bookings\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7A86CC-3006-4AED-980D-545065064A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>CR-ID</t>
   </si>
@@ -256,11 +257,17 @@
 Car-TC-AdminHomePage-004
 Car-TC-AdminHomePage-005</t>
   </si>
+  <si>
+    <t>from
+Car-TC-login-001
+to 
+Car-TC-login-010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -386,40 +393,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,23 +642,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,504 +679,506 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="30">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.8">
+      <c r="A3" s="11"/>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.4">
+      <c r="A4" s="11"/>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4">
+      <c r="A5" s="11"/>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.4">
+      <c r="A6" s="11"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.4">
+      <c r="A7" s="11"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4">
+      <c r="A8" s="11"/>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.4">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.4">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.4">
+      <c r="A11" s="11"/>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.4">
+      <c r="A12" s="11"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.4">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="36" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="16"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="3"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="3"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="3"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="3"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="3"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="3"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="3"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="8" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="3"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="2"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="2"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="2"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A38" s="7"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="8" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" ht="23.25" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2" t="s">
+      <c r="E40" s="9"/>
+      <c r="F40" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="8" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="8" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="45" spans="1:6" ht="15.75" customHeight="1"/>
@@ -2111,20 +2120,10 @@
     <row r="981" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F24:F30"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="E24:E30"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A32:A38"/>
     <mergeCell ref="A40:A43"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D10:D13"/>
@@ -2141,10 +2140,20 @@
     <mergeCell ref="D24:D30"/>
     <mergeCell ref="D32:D38"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="E24:E30"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modify the traceability matrix
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix .xlsx
+++ b/Monitor and Control/Car-Traceability Matrix .xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Car System\Github\Car-Bookings\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eslam\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7A86CC-3006-4AED-980D-545065064A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
   <si>
     <t>CR-ID</t>
-  </si>
-  <si>
-    <t>SR-ID</t>
   </si>
   <si>
     <t>SIQ-ID</t>
@@ -258,17 +254,66 @@
 Car-TC-AdminHomePage-005</t>
   </si>
   <si>
-    <t>from
-Car-TC-login-001
+    <t>Remove search for a car feature</t>
+  </si>
+  <si>
+    <t>CR-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR_Des_Search_002 </t>
+  </si>
+  <si>
+    <t>Req-Regs-001
 to 
+Req-Regs-006</t>
+  </si>
+  <si>
+    <t>Car-TC-login-002
+Car-TC-login-005
+Car-TC-login-006
+Car-TC-login-008
 Car-TC-login-010</t>
+  </si>
+  <si>
+    <t>Car-TC-login-001
+Car-TC-login-003
+Car-TC-login-004
+Car-TC-login-007
+Car-TC-login-009</t>
+  </si>
+  <si>
+    <t>SQ_Admin_AddAdmin_07_ Delete Car (flow chart)</t>
+  </si>
+  <si>
+    <t>CR-009</t>
+  </si>
+  <si>
+    <t>CR-010</t>
+  </si>
+  <si>
+    <t>Impact Analysis</t>
+  </si>
+  <si>
+    <t>SRS-ID</t>
+  </si>
+  <si>
+    <t>SQ_Admin_AddAdmin_02_ AddUser (flow chart)</t>
+  </si>
+  <si>
+    <t>SQ_Admin_AddAdmin_03_ AddAdmin (flow chart)</t>
+  </si>
+  <si>
+    <t>Remove Add admin from Features according to the customer request</t>
+  </si>
+  <si>
+    <t>change_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +346,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -329,13 +380,6 @@
     </fill>
   </fills>
   <borders count="5">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
     <border>
       <left/>
       <right/>
@@ -384,49 +428,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,565 +712,767 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F981"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E13"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" customHeight="1">
+      <c r="A16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G25" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A33" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.8">
-      <c r="A3" s="11"/>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="14.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" ht="14.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="14.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="14.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.4">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.4">
-      <c r="A10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C33" s="11"/>
+      <c r="D33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+      <c r="G33" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="23.25" customHeight="1">
+      <c r="A41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A46" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.4">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="36" customHeight="1">
-      <c r="A15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A38" s="11"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="23.25" customHeight="1">
-      <c r="A40" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9" t="s">
+      <c r="B46" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A43" s="11"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+      <c r="F46" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A51" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A57" s="10"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A59" s="10"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2118,42 +2390,77 @@
     <row r="979" ht="15.75" customHeight="1"/>
     <row r="980" ht="15.75" customHeight="1"/>
     <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A17:C17"/>
+  <mergeCells count="65">
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="G51:G54"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="F56:F59"/>
+    <mergeCell ref="G56:G59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A9:E9"/>
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D24:D30"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="E24:E30"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G33:G39"/>
+    <mergeCell ref="G41:G44"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="F41:F44"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="F33:F39"/>
     <mergeCell ref="F2:F8"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add TCs traceability matrix
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix .xlsx
+++ b/Monitor and Control/Car-Traceability Matrix .xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Car-Bookings\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="117">
   <si>
     <t>CR-ID</t>
   </si>
@@ -59,11 +59,6 @@
 Car - Registration(flow chart)</t>
   </si>
   <si>
-    <t>Req-Regs-001
-to 
-Req-Regs-006</t>
-  </si>
-  <si>
     <t>SIQ-001
 SIQ-009</t>
   </si>
@@ -103,14 +98,6 @@
   <si>
     <t>SQ_User_Login_02
 Car - Login(flow chart)</t>
-  </si>
-  <si>
-    <t>Car-TC-login-001
-Car-TC-login-003
-Car-TC-login-004
-Car-TC-login-007
-Car-TC-login-009
-Car-TC-UserHomePage-001</t>
   </si>
   <si>
     <t>Req-User-Log-002</t>
@@ -156,14 +143,6 @@
   <si>
     <t>SQ_Admin_Login_01
 Car - Login(flow chart)</t>
-  </si>
-  <si>
-    <t>Car-TC-AdminHomePage-001
-Car-TC-login-002
-Car-TC-login-005
-Car-TC-login-006
-Car-TC-login-008
-Car-TC-login-010</t>
   </si>
   <si>
     <t>Req-Admin-log-002</t>
@@ -348,12 +327,123 @@
 to
 Car-Bug-AddCar-002</t>
   </si>
+  <si>
+    <t>Car-TC-Reg-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-Reg-001
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-Reg-001
+Car-TC-Reg-007
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-Reg-001
+Car-TC-Reg-008
+</t>
+  </si>
+  <si>
+    <t>Req-Regs-009</t>
+  </si>
+  <si>
+    <t>Req-Regs-008</t>
+  </si>
+  <si>
+    <t>Car-TC-Reg-009</t>
+  </si>
+  <si>
+    <t>TCs from
+ Car-TC-Reg-001
+To 
+Car-TC-Reg-018</t>
+  </si>
+  <si>
+    <t>From Car-TC-Reg-002 
+to Car-TC-Reg-006
+Car-TC-Reg-008
+From Car-TC-Reg-010
+too Car-TC-Reg-016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-login-001
+</t>
+  </si>
+  <si>
+    <t>Req-User-Log-005</t>
+  </si>
+  <si>
+    <t>Req-User-Log-006</t>
+  </si>
+  <si>
+    <t>Car-TC-UserHomePage-001</t>
+  </si>
+  <si>
+    <t>Car-TC-login-001
+Car-TC-login-002
+Car-TC-login-003
+Car-TC-login-004
+Car-TC-login-005
+Car-TC-login-006
+Car-TC-login-007</t>
+  </si>
+  <si>
+    <t>Car-TC-login-013</t>
+  </si>
+  <si>
+    <t>Car-TC-login-002
+Car-TC-login-005</t>
+  </si>
+  <si>
+    <t>Car-TC-Reg-001
+Car-TC-Reg-003</t>
+  </si>
+  <si>
+    <t>Car-TC-login-002
+Car-TC-login-012</t>
+  </si>
+  <si>
+    <t>Req-Admin-log-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-login-001
+Car-TC-login-012
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-AdminHomePage-001
+Car-TC-login-002
+</t>
+  </si>
+  <si>
+    <t>Car-TC-login-002</t>
+  </si>
+  <si>
+    <t>Car-TC-login-005
+Car-TC-login-006
+Car-TC-login-008
+Car-TC-login-010
+Car-TC-login-011
+Car-TC-login-014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-Reg-001  (Bug_Reg_001)
+Car-TC-Reg-009  (Bug_Reg_003)
+Car-TC-Reg-014  (Bug_Reg_002)
+Car-TC-Reg-018  (Bug_Reg_004)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Car-TC-login-013  (Bug_login_001)
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +487,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -544,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,59 +711,101 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -878,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I987"/>
+  <dimension ref="A1:I991"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26:I32"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -890,7 +1035,8 @@
     <col min="1" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="9" width="26.28515625" customWidth="1"/>
+    <col min="7" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" customWidth="1"/>
     <col min="10" max="28" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -899,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -923,909 +1069,1000 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="35.25" customHeight="1">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:9" ht="36.75" customHeight="1">
+      <c r="A2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
+      <c r="A3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="26"/>
-    </row>
-    <row r="3" spans="1:9" ht="30">
-      <c r="A3" s="42"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="42"/>
+    </row>
+    <row r="4" spans="1:9" ht="45">
+      <c r="A4" s="31"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="42"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="5" spans="1:9" ht="45">
+      <c r="A5" s="31"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="42"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="42"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="42"/>
+    </row>
+    <row r="6" spans="1:9" ht="60">
+      <c r="A6" s="31"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="42"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="42"/>
+    </row>
+    <row r="7" spans="1:9" ht="75">
+      <c r="A7" s="31"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="31"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="42"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="42"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="31"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="33"/>
+      <c r="H9" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="31"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="43"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" customHeight="1">
+      <c r="A12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="26" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="H12" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="38.25" customHeight="1">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="G13" s="32"/>
+      <c r="H13" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="G14" s="32"/>
+      <c r="H14" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="4" t="s">
+      <c r="G15" s="32"/>
+      <c r="H15" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16" spans="1:9" ht="105">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" ht="36" customHeight="1">
+      <c r="A19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="36" customHeight="1">
-      <c r="A16" s="42" t="s">
+      <c r="G19" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="H19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A20" s="44"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="G20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+    </row>
+    <row r="21" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A21" s="7"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A17" s="36"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3" t="s">
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A23" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-    </row>
-    <row r="18" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10" t="s">
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A20" s="42" t="s">
+      <c r="G23" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="H23" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" s="61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5" customHeight="1">
+      <c r="A24" s="31"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G24" s="40"/>
+      <c r="H24" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="1:9" ht="45.75" customHeight="1">
+      <c r="A25" s="31"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="G25" s="40"/>
+      <c r="H25" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A26" s="31"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="29"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="42"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="G26" s="40"/>
+      <c r="H26" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9" ht="102.75" customHeight="1">
+      <c r="A27" s="31"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="42"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="F27" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="42"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="4" t="s">
+      <c r="G27" s="40"/>
+      <c r="H27" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28" spans="1:9" ht="27.75" customHeight="1">
+      <c r="A28" s="31"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="F28" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="40"/>
+      <c r="H28" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A30" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-    </row>
-    <row r="24" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A24" s="42"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="3" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="42" t="s">
+      <c r="G30" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="4" t="s">
+      <c r="H30" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G31" s="33"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A32" s="31"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="4" t="s">
+      <c r="G32" s="33"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A33" s="31"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="42"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="42"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="42"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="42"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="42"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A34" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="26"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>62</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G34" s="33"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A35" s="42"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="33"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A36" s="31"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="33"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A38" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="32"/>
+      <c r="E38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A40" s="31"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A41" s="31"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A36" s="42"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="4" t="s">
+      <c r="G41" s="33"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A42" s="31"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G42" s="33"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A43" s="31"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="28"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A37" s="42"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="G43" s="33"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A44" s="31"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A38" s="42"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="4" t="s">
+      <c r="G44" s="33"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A46" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="42"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="4" t="s">
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A40" s="42"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="4" t="s">
+      <c r="G46" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-    </row>
-    <row r="42" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A42" s="42" t="s">
+      <c r="H46" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="4" t="s">
+      <c r="I46" s="32"/>
+    </row>
+    <row r="47" spans="1:9" ht="29.25" customHeight="1">
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G42" s="26" t="s">
+      <c r="G47" s="33"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="26" t="s">
+      <c r="G48" s="33"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+    </row>
+    <row r="49" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A49" s="44"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I42" s="26"/>
-    </row>
-    <row r="43" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A43" s="42"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="G49" s="50"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+    </row>
+    <row r="50" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G43" s="28"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-    </row>
-    <row r="44" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A44" s="42"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="4" t="s">
+      <c r="G50" s="20"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A52" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="28"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-    </row>
-    <row r="45" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A45" s="36"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="4" t="s">
+      <c r="B52" s="32"/>
+      <c r="C52" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="31"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19" t="s">
+      <c r="D52" s="41"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="22"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A47" s="44"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A48" s="42" t="s">
+      <c r="G52" s="51"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A53" s="31"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A57" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26" t="s">
+      <c r="B57" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36" t="s">
+      <c r="E57" s="46"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A58" s="31"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A59" s="31"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A60" s="31"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A62" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A49" s="42"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A50" s="42"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A51" s="42"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A53" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="35"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="32" t="s">
+      <c r="C62" s="32"/>
+      <c r="D62" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" s="46"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A63" s="31"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A64" s="31"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+    </row>
+    <row r="65" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A65" s="31"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A66" s="36"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+    </row>
+    <row r="67" spans="1:9" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A67" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A54" s="42"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A55" s="42"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A56" s="42"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A58" s="42" t="s">
+      <c r="B67" s="25"/>
+      <c r="C67" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="35"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="32" t="s">
+      <c r="D67" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A59" s="42"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A60" s="42"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-    </row>
-    <row r="61" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A61" s="42"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-    </row>
-    <row r="62" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="24"/>
-    </row>
-    <row r="63" spans="1:9" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="25" t="s">
+      <c r="F67" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="F63" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="69" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="70" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="71" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="73" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="74" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -2733,94 +2970,95 @@
     <row r="985" ht="15.75" customHeight="1"/>
     <row r="986" ht="15.75" customHeight="1"/>
     <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="86">
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="D26:D32"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="F53:F56"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="G26:G32"/>
-    <mergeCell ref="G34:G40"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="H2:H8"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="H26:H32"/>
-    <mergeCell ref="H34:H40"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="H48:H51"/>
-    <mergeCell ref="H53:H56"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="I26:I32"/>
-    <mergeCell ref="I34:I40"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="I53:I56"/>
-    <mergeCell ref="I58:I61"/>
+  <mergeCells count="83">
+    <mergeCell ref="I38:I44"/>
+    <mergeCell ref="I46:I49"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I62:I65"/>
+    <mergeCell ref="I2:I10"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I23:I28"/>
+    <mergeCell ref="I30:I36"/>
+    <mergeCell ref="H38:H44"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H30:H36"/>
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="G30:G36"/>
+    <mergeCell ref="G38:G44"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="C30:C36"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="D38:D44"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="D30:D36"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="D52:D55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update TCs and Bug report
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Traceability Matrix .xlsx
+++ b/Monitor and Control/Car-Traceability Matrix .xlsx
@@ -338,15 +338,15 @@
   </si>
   <si>
     <t>from 
-Car-Bug-AddCar-001
-to
-Car-Bug-AddCar-004</t>
-  </si>
-  <si>
-    <t>from 
 Car-TC-AddCar-001 
 to 
 Car-TC-AddCar-012</t>
+  </si>
+  <si>
+    <t>from 
+Car-Bug-AddCar-001
+to
+Car-Bug-AddCar-002</t>
   </si>
 </sst>
 </file>
@@ -601,67 +601,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,9 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -924,215 +924,215 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="35.25" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="30">
-      <c r="A3" s="34"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="34"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="34"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="34"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="34"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="34"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" ht="36" customHeight="1">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="29"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
@@ -1147,22 +1147,22 @@
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A17" s="35"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="36"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" ht="33.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="28"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="10" t="s">
@@ -1173,18 +1173,18 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="42" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="29"/>
@@ -1205,383 +1205,383 @@
       <c r="I20" s="29"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="34"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="34"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="30"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="H26" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I26" s="29" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="26"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="26"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="26"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="15"/>
       <c r="F32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="26"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="25"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I34" s="25" t="s">
+      <c r="I34" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
       <c r="E35" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="26"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
       <c r="E37" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="26"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="34"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="26"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="15"/>
       <c r="F40" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G40" s="26"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G42" s="25" t="s">
+      <c r="G42" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="I42" s="25"/>
+      <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G43" s="26"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A44" s="34"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="16"/>
       <c r="F44" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="26"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A45" s="35"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="15"/>
       <c r="F45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="42"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" ht="24.75" customHeight="1">
       <c r="A46" s="7"/>
@@ -1597,191 +1597,191 @@
       <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25" t="s">
+      <c r="B48" s="26"/>
+      <c r="C48" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="35" t="s">
+      <c r="D48" s="27"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="43"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A49" s="34"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A50" s="34"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
+      <c r="A50" s="42"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A51" s="34"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
+      <c r="A51" s="42"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
+      <c r="A52" s="43"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25" t="s">
+      <c r="C53" s="26"/>
+      <c r="D53" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="E53" s="38"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="43" t="s">
+      <c r="E53" s="35"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A54" s="34"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
+      <c r="A54" s="42"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A55" s="34"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
+      <c r="A55" s="42"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A56" s="34"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
+      <c r="A56" s="42"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25" t="s">
+      <c r="C58" s="26"/>
+      <c r="D58" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="E58" s="38"/>
+      <c r="E58" s="35"/>
       <c r="F58" s="41"/>
-      <c r="G58" s="43" t="s">
+      <c r="G58" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A59" s="34"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="25"/>
+      <c r="A59" s="42"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A60" s="34"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="25"/>
+      <c r="A60" s="42"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A61" s="34"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="25"/>
+      <c r="A61" s="42"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1">
       <c r="A62" s="45"/>
@@ -1790,22 +1790,22 @@
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
       <c r="F62" s="45"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="46"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
     </row>
     <row r="63" spans="1:9" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="47"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D63" s="47" t="s">
+      <c r="D63" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F63" s="47" t="s">
+      <c r="F63" s="25" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2735,47 +2735,35 @@
     <row r="987" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="I34:I40"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="I53:I56"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="I26:I32"/>
-    <mergeCell ref="H34:H40"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="H48:H51"/>
-    <mergeCell ref="H53:H56"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="H2:H8"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="H26:H32"/>
-    <mergeCell ref="G34:G40"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="G26:G32"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="F53:F56"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="D34:D40"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="D26:D32"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="C2:C8"/>
@@ -2792,35 +2780,47 @@
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="A57:F57"/>
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="D26:D32"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D34:D40"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="F53:F56"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="G26:G32"/>
+    <mergeCell ref="G34:G40"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="H26:H32"/>
+    <mergeCell ref="H34:H40"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="H53:H56"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="I2:I8"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="I26:I32"/>
+    <mergeCell ref="I34:I40"/>
+    <mergeCell ref="I42:I45"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="I53:I56"/>
+    <mergeCell ref="I58:I61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>